<commit_message>
added a few more colmns and edits
</commit_message>
<xml_diff>
--- a/notebooks/exp_a.xlsx
+++ b/notebooks/exp_a.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S149"/>
+  <dimension ref="A1:U149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,16 @@
           <t>exp_current_arra</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>city/state</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>exp_per_student</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -598,6 +608,14 @@
       <c r="S2" t="n">
         <v>0</v>
       </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Nashville, TN</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>19316.2923231646</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -667,6 +685,14 @@
       <c r="S3" t="n">
         <v>0</v>
       </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Alamo, TN</t>
+        </is>
+      </c>
+      <c r="U3" t="n">
+        <v>9494.809688581316</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -733,6 +759,14 @@
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="n">
         <v>0</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Alcoa, TN</t>
+        </is>
+      </c>
+      <c r="U4" t="n">
+        <v>11587.51696065129</v>
       </c>
     </row>
     <row r="5">
@@ -779,6 +813,12 @@
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Jamestown, TN</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -848,6 +888,14 @@
       <c r="S6" t="n">
         <v>0</v>
       </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Clinton, TN</t>
+        </is>
+      </c>
+      <c r="U6" t="n">
+        <v>11690.67595377553</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -915,6 +963,14 @@
         <v>408000</v>
       </c>
       <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Arlington, TN</t>
+        </is>
+      </c>
+      <c r="U7" t="n">
+        <v>10295.23214657506</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -984,6 +1040,14 @@
       <c r="S8" t="n">
         <v>0</v>
       </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Athens, TN</t>
+        </is>
+      </c>
+      <c r="U8" t="n">
+        <v>10234.73917869034</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1051,6 +1115,14 @@
         <v>84000</v>
       </c>
       <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Bartlett, TN</t>
+        </is>
+      </c>
+      <c r="U9" t="n">
+        <v>13881.28772635815</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1120,6 +1192,14 @@
       <c r="S10" t="n">
         <v>0</v>
       </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Shelbyville, TN</t>
+        </is>
+      </c>
+      <c r="U10" t="n">
+        <v>10234.88449209683</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1187,6 +1267,14 @@
       <c r="S11" t="n">
         <v>0</v>
       </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Bells, TN</t>
+        </is>
+      </c>
+      <c r="U11" t="n">
+        <v>9619.047619047618</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1256,6 +1344,14 @@
       <c r="S12" t="n">
         <v>0</v>
       </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Camden, TN</t>
+        </is>
+      </c>
+      <c r="U12" t="n">
+        <v>10666.66666666667</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1325,6 +1421,14 @@
       <c r="S13" t="n">
         <v>0</v>
       </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Pikeville, TN</t>
+        </is>
+      </c>
+      <c r="U13" t="n">
+        <v>11609.43168077388</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1394,6 +1498,14 @@
       <c r="S14" t="n">
         <v>0</v>
       </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Maryville, TN</t>
+        </is>
+      </c>
+      <c r="U14" t="n">
+        <v>10765.38987688098</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1461,6 +1573,14 @@
       <c r="S15" t="n">
         <v>0</v>
       </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Bradford, TN</t>
+        </is>
+      </c>
+      <c r="U15" t="n">
+        <v>10128.45528455285</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1530,6 +1650,14 @@
       <c r="S16" t="n">
         <v>0</v>
       </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Cleveland, TN</t>
+        </is>
+      </c>
+      <c r="U16" t="n">
+        <v>9240.919271594119</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1599,6 +1727,14 @@
       <c r="S17" t="n">
         <v>0</v>
       </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Bristol, TN</t>
+        </is>
+      </c>
+      <c r="U17" t="n">
+        <v>11053.36311739886</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1668,6 +1804,14 @@
       <c r="S18" t="n">
         <v>0</v>
       </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Jacksboro, TN</t>
+        </is>
+      </c>
+      <c r="U18" t="n">
+        <v>10171.32602946732</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1737,6 +1881,14 @@
       <c r="S19" t="n">
         <v>0</v>
       </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Woodbury, TN</t>
+        </is>
+      </c>
+      <c r="U19" t="n">
+        <v>10413.94101876676</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1806,6 +1958,14 @@
       <c r="S20" t="n">
         <v>0</v>
       </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Huntingdon, TN</t>
+        </is>
+      </c>
+      <c r="U20" t="n">
+        <v>1700000</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1875,6 +2035,14 @@
       <c r="S21" t="n">
         <v>0</v>
       </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Elizabethton, TN</t>
+        </is>
+      </c>
+      <c r="U21" t="n">
+        <v>11268.05205709488</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1944,6 +2112,14 @@
       <c r="S22" t="n">
         <v>0</v>
       </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Ashland City, TN</t>
+        </is>
+      </c>
+      <c r="U22" t="n">
+        <v>10216.01234356249</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2013,6 +2189,14 @@
       <c r="S23" t="n">
         <v>0</v>
       </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Henderson, TN</t>
+        </is>
+      </c>
+      <c r="U23" t="n">
+        <v>9787.620064034152</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2082,6 +2266,14 @@
       <c r="S24" t="n">
         <v>0</v>
       </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Tazewell, TN</t>
+        </is>
+      </c>
+      <c r="U24" t="n">
+        <v>10324.07862407862</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2151,6 +2343,14 @@
       <c r="S25" t="n">
         <v>0</v>
       </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Celina, TN</t>
+        </is>
+      </c>
+      <c r="U25" t="n">
+        <v>10570.64721969006</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2220,6 +2420,14 @@
       <c r="S26" t="n">
         <v>0</v>
       </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>Cleveland, TN</t>
+        </is>
+      </c>
+      <c r="U26" t="n">
+        <v>11259.18862690707</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2287,6 +2495,14 @@
       <c r="S27" t="n">
         <v>0</v>
       </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Clinton, TN</t>
+        </is>
+      </c>
+      <c r="U27" t="n">
+        <v>9934.917355371901</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2356,6 +2572,14 @@
       <c r="S28" t="n">
         <v>0</v>
       </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>Newport, TN</t>
+        </is>
+      </c>
+      <c r="U28" t="n">
+        <v>10513.4823692095</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2425,6 +2649,14 @@
       <c r="S29" t="n">
         <v>0</v>
       </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>Manchester, TN</t>
+        </is>
+      </c>
+      <c r="U29" t="n">
+        <v>10799.31740614335</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2492,6 +2724,14 @@
         <v>171000</v>
       </c>
       <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>Collierville, TN</t>
+        </is>
+      </c>
+      <c r="U30" t="n">
+        <v>11844.79965439032</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2561,6 +2801,14 @@
       <c r="S31" t="n">
         <v>0</v>
       </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>Alamo, TN</t>
+        </is>
+      </c>
+      <c r="U31" t="n">
+        <v>9507.485029940121</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2630,6 +2878,14 @@
       <c r="S32" t="n">
         <v>0</v>
       </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>Crossville, TN</t>
+        </is>
+      </c>
+      <c r="U32" t="n">
+        <v>9306.541019955654</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2699,6 +2955,14 @@
       <c r="S33" t="n">
         <v>0</v>
       </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>Nashville, TN</t>
+        </is>
+      </c>
+      <c r="U33" t="n">
+        <v>14857.12514413956</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2766,6 +3030,14 @@
       <c r="S34" t="n">
         <v>0</v>
       </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>Dayton, TN</t>
+        </is>
+      </c>
+      <c r="U34" t="n">
+        <v>9713.443396226416</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2833,6 +3105,14 @@
       <c r="S35" t="n">
         <v>0</v>
       </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>Decaturville, TN</t>
+        </is>
+      </c>
+      <c r="U35" t="n">
+        <v>10301.1811023622</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2901,6 +3181,14 @@
       </c>
       <c r="S36" t="n">
         <v>0</v>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>Smithville, TN</t>
+        </is>
+      </c>
+      <c r="U36" t="n">
+        <v>8852.280462899931</v>
       </c>
     </row>
     <row r="37">
@@ -2947,6 +3235,12 @@
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
       <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>Nashville, TN</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3016,6 +3310,14 @@
       <c r="S38" t="n">
         <v>0</v>
       </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>Dickson, TN</t>
+        </is>
+      </c>
+      <c r="U38" t="n">
+        <v>9875.753475212203</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3085,6 +3387,14 @@
       <c r="S39" t="n">
         <v>0</v>
       </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>Dyersburg, TN</t>
+        </is>
+      </c>
+      <c r="U39" t="n">
+        <v>10886.14540466392</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3152,6 +3462,14 @@
       <c r="S40" t="n">
         <v>0</v>
       </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>Dyersburg, TN</t>
+        </is>
+      </c>
+      <c r="U40" t="n">
+        <v>11401.45426712591</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3221,6 +3539,14 @@
       <c r="S41" t="n">
         <v>0</v>
       </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>Elizabethton, TN</t>
+        </is>
+      </c>
+      <c r="U41" t="n">
+        <v>10092.7684441198</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3288,6 +3614,14 @@
       <c r="S42" t="n">
         <v>0</v>
       </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>Etowah, TN</t>
+        </is>
+      </c>
+      <c r="U42" t="n">
+        <v>10274.05247813411</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3357,6 +3691,14 @@
       <c r="S43" t="n">
         <v>0</v>
       </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>Somerville, TN</t>
+        </is>
+      </c>
+      <c r="U43" t="n">
+        <v>10643.29833230389</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3426,6 +3768,14 @@
       <c r="S44" t="n">
         <v>0</v>
       </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>Fayetteville, TN</t>
+        </is>
+      </c>
+      <c r="U44" t="n">
+        <v>11798.31223628692</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3493,6 +3843,14 @@
       <c r="S45" t="n">
         <v>0</v>
       </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>Jamestown, TN</t>
+        </is>
+      </c>
+      <c r="U45" t="n">
+        <v>9446.69603524229</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3562,6 +3920,14 @@
       <c r="S46" t="n">
         <v>0</v>
       </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>Winchester, TN</t>
+        </is>
+      </c>
+      <c r="U46" t="n">
+        <v>10948.6410871303</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -3631,6 +3997,14 @@
       <c r="S47" t="n">
         <v>0</v>
       </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>Franklin, TN</t>
+        </is>
+      </c>
+      <c r="U47" t="n">
+        <v>19254.54545454546</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -3698,6 +4072,14 @@
         <v>129000</v>
       </c>
       <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>Germantown, TN</t>
+        </is>
+      </c>
+      <c r="U48" t="n">
+        <v>14181.04878858281</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -3767,6 +4149,14 @@
       <c r="S49" t="n">
         <v>0</v>
       </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>Dyer, TN</t>
+        </is>
+      </c>
+      <c r="U49" t="n">
+        <v>9109.793033821303</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -3836,6 +4226,14 @@
       <c r="S50" t="n">
         <v>0</v>
       </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>Pulaski, TN</t>
+        </is>
+      </c>
+      <c r="U50" t="n">
+        <v>10205.17711171662</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -3905,6 +4303,14 @@
       <c r="S51" t="n">
         <v>0</v>
       </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>Rutledge, TN</t>
+        </is>
+      </c>
+      <c r="U51" t="n">
+        <v>11323.67149758454</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3972,6 +4378,14 @@
       <c r="S52" t="n">
         <v>0</v>
       </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>Greeneville, TN</t>
+        </is>
+      </c>
+      <c r="U52" t="n">
+        <v>10380.526735834</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -4041,6 +4455,14 @@
       <c r="S53" t="n">
         <v>0</v>
       </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>Greeneville, TN</t>
+        </is>
+      </c>
+      <c r="U53" t="n">
+        <v>11125.79245912579</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -4110,6 +4532,14 @@
       <c r="S54" t="n">
         <v>0</v>
       </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>Altamont, TN</t>
+        </is>
+      </c>
+      <c r="U54" t="n">
+        <v>11361.65455561766</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -4179,6 +4609,14 @@
       <c r="S55" t="n">
         <v>0</v>
       </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>Morristown, TN</t>
+        </is>
+      </c>
+      <c r="U55" t="n">
+        <v>10058.1203226747</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -4248,6 +4686,14 @@
       <c r="S56" t="n">
         <v>0</v>
       </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>Chattanooga, TN</t>
+        </is>
+      </c>
+      <c r="U56" t="n">
+        <v>10453.42250882315</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -4315,6 +4761,14 @@
       <c r="S57" t="n">
         <v>0</v>
       </c>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>Sneedville, TN</t>
+        </is>
+      </c>
+      <c r="U57" t="n">
+        <v>11327.04402515723</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -4384,6 +4838,14 @@
       <c r="S58" t="n">
         <v>0</v>
       </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>Bolivar, TN</t>
+        </is>
+      </c>
+      <c r="U58" t="n">
+        <v>12308.22328931573</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -4453,6 +4915,14 @@
       <c r="S59" t="n">
         <v>0</v>
       </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>Savannah, TN</t>
+        </is>
+      </c>
+      <c r="U59" t="n">
+        <v>10778.04154302671</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -4522,6 +4992,14 @@
       <c r="S60" t="n">
         <v>0</v>
       </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>Rogersville, TN</t>
+        </is>
+      </c>
+      <c r="U60" t="n">
+        <v>11189.40355329949</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -4590,6 +5068,14 @@
       </c>
       <c r="S61" t="n">
         <v>0</v>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>Brownsville, TN</t>
+        </is>
+      </c>
+      <c r="U61" t="n">
+        <v>11068.72473355384</v>
       </c>
     </row>
     <row r="62">
@@ -4658,6 +5144,14 @@
       <c r="S62" t="n">
         <v>0</v>
       </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>Lexington, TN</t>
+        </is>
+      </c>
+      <c r="U62" t="n">
+        <v>9444.745929945733</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -4725,6 +5219,14 @@
       <c r="S63" t="n">
         <v>0</v>
       </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>Paris, TN</t>
+        </is>
+      </c>
+      <c r="U63" t="n">
+        <v>10746.84804246848</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -4794,6 +5296,14 @@
       <c r="S64" t="n">
         <v>0</v>
       </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>Centerville, TN</t>
+        </is>
+      </c>
+      <c r="U64" t="n">
+        <v>10755.5905511811</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -4863,6 +5373,14 @@
       <c r="S65" t="n">
         <v>0</v>
       </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>Bruceton, TN</t>
+        </is>
+      </c>
+      <c r="U65" t="n">
+        <v>9325.227963525836</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -4932,6 +5450,14 @@
       <c r="S66" t="n">
         <v>0</v>
       </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>Erin, TN</t>
+        </is>
+      </c>
+      <c r="U66" t="n">
+        <v>10471.50663544106</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -5001,6 +5527,14 @@
       <c r="S67" t="n">
         <v>0</v>
       </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>Humboldt, TN</t>
+        </is>
+      </c>
+      <c r="U67" t="n">
+        <v>12778.37837837838</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -5070,6 +5604,14 @@
       <c r="S68" t="n">
         <v>0</v>
       </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>Waverly, TN</t>
+        </is>
+      </c>
+      <c r="U68" t="n">
+        <v>10383.58707760862</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5137,6 +5679,14 @@
       <c r="S69" t="n">
         <v>0</v>
       </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>Huntingdon, TN</t>
+        </is>
+      </c>
+      <c r="U69" t="n">
+        <v>9847.940074906366</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5204,6 +5754,14 @@
       <c r="S70" t="n">
         <v>0</v>
       </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>Gainesboro, TN</t>
+        </is>
+      </c>
+      <c r="U70" t="n">
+        <v>10634.996582365</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -5273,6 +5831,14 @@
       <c r="S71" t="n">
         <v>0</v>
       </c>
+      <c r="T71" t="inlineStr">
+        <is>
+          <t>Dandridge, TN</t>
+        </is>
+      </c>
+      <c r="U71" t="n">
+        <v>10087.06218727663</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -5342,6 +5908,14 @@
       <c r="S72" t="n">
         <v>0</v>
       </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>Johnson City, TN</t>
+        </is>
+      </c>
+      <c r="U72" t="n">
+        <v>10494.31321084864</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -5411,6 +5985,14 @@
       <c r="S73" t="n">
         <v>0</v>
       </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>Mountain City, TN</t>
+        </is>
+      </c>
+      <c r="U73" t="n">
+        <v>4570.911285455642</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -5480,6 +6062,14 @@
       <c r="S74" t="n">
         <v>0</v>
       </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>Kingsport, TN</t>
+        </is>
+      </c>
+      <c r="U74" t="n">
+        <v>10683.96711202467</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -5549,6 +6139,14 @@
       <c r="S75" t="n">
         <v>0</v>
       </c>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>Knoxville, TN</t>
+        </is>
+      </c>
+      <c r="U75" t="n">
+        <v>9621.524856044482</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -5618,6 +6216,14 @@
       <c r="S76" t="n">
         <v>0</v>
       </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>Tiptonville, TN</t>
+        </is>
+      </c>
+      <c r="U76" t="n">
+        <v>14710.28037383178</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -5685,6 +6291,14 @@
         <v>2000</v>
       </c>
       <c r="S77" t="inlineStr"/>
+      <c r="T77" t="inlineStr">
+        <is>
+          <t>Lakeland, TN</t>
+        </is>
+      </c>
+      <c r="U77" t="n">
+        <v>11061.44465290807</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -5752,6 +6366,14 @@
       <c r="S78" t="n">
         <v>0</v>
       </c>
+      <c r="T78" t="inlineStr">
+        <is>
+          <t>Ripley, TN</t>
+        </is>
+      </c>
+      <c r="U78" t="n">
+        <v>12655.14210372107</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -5821,6 +6443,14 @@
       <c r="S79" t="n">
         <v>0</v>
       </c>
+      <c r="T79" t="inlineStr">
+        <is>
+          <t>Lawrenceburg, TN</t>
+        </is>
+      </c>
+      <c r="U79" t="n">
+        <v>9458.902161547212</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -5890,6 +6520,14 @@
       <c r="S80" t="n">
         <v>0</v>
       </c>
+      <c r="T80" t="inlineStr">
+        <is>
+          <t>Lebanon, TN</t>
+        </is>
+      </c>
+      <c r="U80" t="n">
+        <v>9670.694148306089</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -5959,6 +6597,14 @@
       <c r="S81" t="n">
         <v>0</v>
       </c>
+      <c r="T81" t="inlineStr">
+        <is>
+          <t>Lenoir City, TN</t>
+        </is>
+      </c>
+      <c r="U81" t="n">
+        <v>10211.05919003115</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -6028,6 +6674,14 @@
       <c r="S82" t="n">
         <v>0</v>
       </c>
+      <c r="T82" t="inlineStr">
+        <is>
+          <t>Hohenwald, TN</t>
+        </is>
+      </c>
+      <c r="U82" t="n">
+        <v>9506.478209658422</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -6097,6 +6751,14 @@
       <c r="S83" t="n">
         <v>0</v>
       </c>
+      <c r="T83" t="inlineStr">
+        <is>
+          <t>Lexington, TN</t>
+        </is>
+      </c>
+      <c r="U83" t="n">
+        <v>10395.92760180996</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -6164,6 +6826,14 @@
       <c r="S84" t="n">
         <v>0</v>
       </c>
+      <c r="T84" t="inlineStr">
+        <is>
+          <t>Fayetteville, TN</t>
+        </is>
+      </c>
+      <c r="U84" t="n">
+        <v>9736.631684157921</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6233,6 +6903,14 @@
       <c r="S85" t="n">
         <v>0</v>
       </c>
+      <c r="T85" t="inlineStr">
+        <is>
+          <t>Loudon, TN</t>
+        </is>
+      </c>
+      <c r="U85" t="n">
+        <v>9917.45330387628</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -6302,6 +6980,14 @@
       <c r="S86" t="n">
         <v>0</v>
       </c>
+      <c r="T86" t="inlineStr">
+        <is>
+          <t>Lafayette, TN</t>
+        </is>
+      </c>
+      <c r="U86" t="n">
+        <v>9007.090522335146</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -6371,6 +7057,14 @@
       <c r="S87" t="n">
         <v>0</v>
       </c>
+      <c r="T87" t="inlineStr">
+        <is>
+          <t>Jackson, TN</t>
+        </is>
+      </c>
+      <c r="U87" t="n">
+        <v>11348.6319505737</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -6440,6 +7134,14 @@
       <c r="S88" t="n">
         <v>0</v>
       </c>
+      <c r="T88" t="inlineStr">
+        <is>
+          <t>Manchester, TN</t>
+        </is>
+      </c>
+      <c r="U88" t="n">
+        <v>11085.91282375237</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -6509,6 +7211,14 @@
       <c r="S89" t="n">
         <v>0</v>
       </c>
+      <c r="T89" t="inlineStr">
+        <is>
+          <t>Jasper, TN</t>
+        </is>
+      </c>
+      <c r="U89" t="n">
+        <v>9828.787878787878</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -6576,6 +7286,14 @@
       <c r="S90" t="n">
         <v>0</v>
       </c>
+      <c r="T90" t="inlineStr">
+        <is>
+          <t>Lewisburg, TN</t>
+        </is>
+      </c>
+      <c r="U90" t="n">
+        <v>9836.662967073622</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -6645,6 +7363,14 @@
       <c r="S91" t="n">
         <v>0</v>
       </c>
+      <c r="T91" t="inlineStr">
+        <is>
+          <t>Maryville, TN</t>
+        </is>
+      </c>
+      <c r="U91" t="n">
+        <v>11460.41262563922</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -6714,6 +7440,14 @@
       <c r="S92" t="n">
         <v>0</v>
       </c>
+      <c r="T92" t="inlineStr">
+        <is>
+          <t>Columbia, TN</t>
+        </is>
+      </c>
+      <c r="U92" t="n">
+        <v>9406.25</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -6783,6 +7517,14 @@
       <c r="S93" t="n">
         <v>0</v>
       </c>
+      <c r="T93" t="inlineStr">
+        <is>
+          <t>McKenzie, TN</t>
+        </is>
+      </c>
+      <c r="U93" t="n">
+        <v>9072.204968944099</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -6849,6 +7591,14 @@
       <c r="R94" t="inlineStr"/>
       <c r="S94" t="n">
         <v>0</v>
+      </c>
+      <c r="T94" t="inlineStr">
+        <is>
+          <t>Athens, TN</t>
+        </is>
+      </c>
+      <c r="U94" t="n">
+        <v>9889.56937799043</v>
       </c>
     </row>
     <row r="95">
@@ -6915,6 +7665,14 @@
       <c r="S95" t="n">
         <v>0</v>
       </c>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>Selmer, TN</t>
+        </is>
+      </c>
+      <c r="U95" t="n">
+        <v>10505.87314017228</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -6984,6 +7742,14 @@
       <c r="S96" t="n">
         <v>0</v>
       </c>
+      <c r="T96" t="inlineStr">
+        <is>
+          <t>Decatur, TN</t>
+        </is>
+      </c>
+      <c r="U96" t="n">
+        <v>9952.598515134208</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -7053,6 +7819,14 @@
       <c r="S97" t="n">
         <v>0</v>
       </c>
+      <c r="T97" t="inlineStr">
+        <is>
+          <t>Memphis, TN</t>
+        </is>
+      </c>
+      <c r="U97" t="n">
+        <v>12974.87180888367</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -7122,6 +7896,14 @@
       <c r="S98" t="n">
         <v>0</v>
       </c>
+      <c r="T98" t="inlineStr">
+        <is>
+          <t>Milan, TN</t>
+        </is>
+      </c>
+      <c r="U98" t="n">
+        <v>10189.87975951904</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -7189,6 +7971,14 @@
         <v>26000</v>
       </c>
       <c r="S99" t="inlineStr"/>
+      <c r="T99" t="inlineStr">
+        <is>
+          <t>Millington, TN</t>
+        </is>
+      </c>
+      <c r="U99" t="n">
+        <v>12653.72790161414</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -7256,6 +8046,14 @@
       <c r="S100" t="n">
         <v>0</v>
       </c>
+      <c r="T100" t="inlineStr">
+        <is>
+          <t>Madisonville, TN</t>
+        </is>
+      </c>
+      <c r="U100" t="n">
+        <v>10627.51343818435</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -7325,6 +8123,14 @@
       <c r="S101" t="n">
         <v>0</v>
       </c>
+      <c r="T101" t="inlineStr">
+        <is>
+          <t>Clarksville, TN</t>
+        </is>
+      </c>
+      <c r="U101" t="n">
+        <v>9484.280298145617</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -7394,6 +8200,14 @@
       <c r="S102" t="n">
         <v>0</v>
       </c>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>Lynchburg, TN</t>
+        </is>
+      </c>
+      <c r="U102" t="n">
+        <v>17865.70477247503</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -7463,6 +8277,14 @@
       <c r="S103" t="n">
         <v>0</v>
       </c>
+      <c r="T103" t="inlineStr">
+        <is>
+          <t>Wartburg, TN</t>
+        </is>
+      </c>
+      <c r="U103" t="n">
+        <v>10379.56204379562</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -7532,6 +8354,14 @@
       <c r="S104" t="n">
         <v>0</v>
       </c>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>Murfreesboro, TN</t>
+        </is>
+      </c>
+      <c r="U104" t="n">
+        <v>9981.079931972788</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -7599,6 +8429,14 @@
       <c r="S105" t="n">
         <v>0</v>
       </c>
+      <c r="T105" t="inlineStr">
+        <is>
+          <t>Newport, TN</t>
+        </is>
+      </c>
+      <c r="U105" t="n">
+        <v>10499.28673323823</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -7668,6 +8506,14 @@
       <c r="S106" t="n">
         <v>0</v>
       </c>
+      <c r="T106" t="inlineStr">
+        <is>
+          <t>Oak Ridge, TN</t>
+        </is>
+      </c>
+      <c r="U106" t="n">
+        <v>13101.39084861923</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -7737,6 +8583,14 @@
       <c r="S107" t="n">
         <v>0</v>
       </c>
+      <c r="T107" t="inlineStr">
+        <is>
+          <t>Union City, TN</t>
+        </is>
+      </c>
+      <c r="U107" t="n">
+        <v>10655.63764857051</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -7804,6 +8658,14 @@
       <c r="S108" t="n">
         <v>0</v>
       </c>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>Oneida, TN</t>
+        </is>
+      </c>
+      <c r="U108" t="n">
+        <v>8509.227614490772</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -7871,6 +8733,14 @@
       <c r="S109" t="n">
         <v>0</v>
       </c>
+      <c r="T109" t="inlineStr">
+        <is>
+          <t>Livingston, TN</t>
+        </is>
+      </c>
+      <c r="U109" t="n">
+        <v>9948.098001289491</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -7938,6 +8808,14 @@
       <c r="S110" t="n">
         <v>0</v>
       </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>Paris, TN</t>
+        </is>
+      </c>
+      <c r="U110" t="n">
+        <v>11311.67192429022</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -8007,6 +8885,14 @@
       <c r="S111" t="n">
         <v>0</v>
       </c>
+      <c r="T111" t="inlineStr">
+        <is>
+          <t>Linden, TN</t>
+        </is>
+      </c>
+      <c r="U111" t="n">
+        <v>11379.79420018709</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -8074,6 +8960,14 @@
       <c r="S112" t="n">
         <v>0</v>
       </c>
+      <c r="T112" t="inlineStr">
+        <is>
+          <t>Byrdstown, TN</t>
+        </is>
+      </c>
+      <c r="U112" t="n">
+        <v>11068.32298136646</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -8141,6 +9035,14 @@
       <c r="S113" t="n">
         <v>0</v>
       </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>Benton, TN</t>
+        </is>
+      </c>
+      <c r="U113" t="n">
+        <v>10704.37616387337</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -8210,6 +9112,14 @@
       <c r="S114" t="n">
         <v>0</v>
       </c>
+      <c r="T114" t="inlineStr">
+        <is>
+          <t>Cookeville, TN</t>
+        </is>
+      </c>
+      <c r="U114" t="n">
+        <v>9605.884308510638</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -8279,6 +9189,14 @@
       <c r="S115" t="n">
         <v>0</v>
       </c>
+      <c r="T115" t="inlineStr">
+        <is>
+          <t>Dayton, TN</t>
+        </is>
+      </c>
+      <c r="U115" t="n">
+        <v>10488.63358592031</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -8348,6 +9266,14 @@
       <c r="S116" t="n">
         <v>0</v>
       </c>
+      <c r="T116" t="inlineStr">
+        <is>
+          <t>South Pittsburg, TN</t>
+        </is>
+      </c>
+      <c r="U116" t="n">
+        <v>14208.79120879121</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -8417,6 +9343,14 @@
       <c r="S117" t="n">
         <v>0</v>
       </c>
+      <c r="T117" t="inlineStr">
+        <is>
+          <t>Kingston, TN</t>
+        </is>
+      </c>
+      <c r="U117" t="n">
+        <v>10490.38461538462</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -8486,6 +9420,14 @@
       <c r="S118" t="n">
         <v>0</v>
       </c>
+      <c r="T118" t="inlineStr">
+        <is>
+          <t>Springfield, TN</t>
+        </is>
+      </c>
+      <c r="U118" t="n">
+        <v>10001.47774687065</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -8555,6 +9497,14 @@
       <c r="S119" t="n">
         <v>0</v>
       </c>
+      <c r="T119" t="inlineStr">
+        <is>
+          <t>Rogersville, TN</t>
+        </is>
+      </c>
+      <c r="U119" t="n">
+        <v>11073.71794871795</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -8624,6 +9574,14 @@
       <c r="S120" t="n">
         <v>0</v>
       </c>
+      <c r="T120" t="inlineStr">
+        <is>
+          <t>Murfreesboro, TN</t>
+        </is>
+      </c>
+      <c r="U120" t="n">
+        <v>10966.25712426292</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -8691,6 +9649,14 @@
       <c r="S121" t="n">
         <v>0</v>
       </c>
+      <c r="T121" t="inlineStr">
+        <is>
+          <t>Huntsville, TN</t>
+        </is>
+      </c>
+      <c r="U121" t="n">
+        <v>11211.96513470681</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -8760,6 +9726,14 @@
       <c r="S122" t="n">
         <v>0</v>
       </c>
+      <c r="T122" t="inlineStr">
+        <is>
+          <t>Dunlap, TN</t>
+        </is>
+      </c>
+      <c r="U122" t="n">
+        <v>10265.8788774003</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -8829,6 +9803,14 @@
       <c r="S123" t="n">
         <v>0</v>
       </c>
+      <c r="T123" t="inlineStr">
+        <is>
+          <t>Sevierville, TN</t>
+        </is>
+      </c>
+      <c r="U123" t="n">
+        <v>11598.61639571083</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -8898,6 +9880,14 @@
       <c r="S124" t="n">
         <v>0</v>
       </c>
+      <c r="T124" t="inlineStr">
+        <is>
+          <t>Carthage, TN</t>
+        </is>
+      </c>
+      <c r="U124" t="n">
+        <v>10213.98235870631</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -8965,6 +9955,14 @@
       <c r="S125" t="n">
         <v>0</v>
       </c>
+      <c r="T125" t="inlineStr">
+        <is>
+          <t>Clarksburg, TN</t>
+        </is>
+      </c>
+      <c r="U125" t="n">
+        <v>10436.92307692308</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -9034,6 +10032,14 @@
       <c r="S126" t="n">
         <v>0</v>
       </c>
+      <c r="T126" t="inlineStr">
+        <is>
+          <t>Dover, TN</t>
+        </is>
+      </c>
+      <c r="U126" t="n">
+        <v>10020.47952047952</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -9103,6 +10109,14 @@
       <c r="S127" t="n">
         <v>0</v>
       </c>
+      <c r="T127" t="inlineStr">
+        <is>
+          <t>Blountville, TN</t>
+        </is>
+      </c>
+      <c r="U127" t="n">
+        <v>11828.99761336515</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -9172,6 +10186,14 @@
       <c r="S128" t="n">
         <v>0</v>
       </c>
+      <c r="T128" t="inlineStr">
+        <is>
+          <t>Gallatin, TN</t>
+        </is>
+      </c>
+      <c r="U128" t="n">
+        <v>9371.534556813745</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -9238,6 +10260,14 @@
       <c r="R129" t="inlineStr"/>
       <c r="S129" t="n">
         <v>0</v>
+      </c>
+      <c r="T129" t="inlineStr">
+        <is>
+          <t>Sweetwater, TN</t>
+        </is>
+      </c>
+      <c r="U129" t="n">
+        <v>8732.166890982504</v>
       </c>
     </row>
     <row r="130">
@@ -9284,6 +10314,12 @@
       <c r="Q130" t="inlineStr"/>
       <c r="R130" t="inlineStr"/>
       <c r="S130" t="inlineStr"/>
+      <c r="T130" t="inlineStr">
+        <is>
+          <t>Nashville, TN</t>
+        </is>
+      </c>
+      <c r="U130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -9329,6 +10365,12 @@
       <c r="Q131" t="inlineStr"/>
       <c r="R131" t="inlineStr"/>
       <c r="S131" t="inlineStr"/>
+      <c r="T131" t="inlineStr">
+        <is>
+          <t>Nashville, TN</t>
+        </is>
+      </c>
+      <c r="U131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -9374,6 +10416,12 @@
       <c r="Q132" t="inlineStr"/>
       <c r="R132" t="inlineStr"/>
       <c r="S132" t="inlineStr"/>
+      <c r="T132" t="inlineStr">
+        <is>
+          <t>Knoxville, TN</t>
+        </is>
+      </c>
+      <c r="U132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -9443,6 +10491,14 @@
       <c r="S133" t="n">
         <v>0</v>
       </c>
+      <c r="T133" t="inlineStr">
+        <is>
+          <t>Covington, TN</t>
+        </is>
+      </c>
+      <c r="U133" t="n">
+        <v>9441.896770416626</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -9512,6 +10568,14 @@
       <c r="S134" t="n">
         <v>0</v>
       </c>
+      <c r="T134" t="inlineStr">
+        <is>
+          <t>Trenton, TN</t>
+        </is>
+      </c>
+      <c r="U134" t="n">
+        <v>12045.79025110783</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -9580,6 +10644,14 @@
       </c>
       <c r="S135" t="n">
         <v>0</v>
+      </c>
+      <c r="T135" t="inlineStr">
+        <is>
+          <t>Hartsville, TN</t>
+        </is>
+      </c>
+      <c r="U135" t="n">
+        <v>9604.122245913291</v>
       </c>
     </row>
     <row r="136">
@@ -9646,6 +10718,14 @@
       <c r="S136" t="n">
         <v>0</v>
       </c>
+      <c r="T136" t="inlineStr">
+        <is>
+          <t>Tullahoma, TN</t>
+        </is>
+      </c>
+      <c r="U136" t="n">
+        <v>10798.13238121395</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -9713,6 +10793,14 @@
       <c r="S137" t="n">
         <v>0</v>
       </c>
+      <c r="T137" t="inlineStr">
+        <is>
+          <t>Erwin, TN</t>
+        </is>
+      </c>
+      <c r="U137" t="n">
+        <v>10745.04504504504</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -9782,6 +10870,14 @@
       <c r="S138" t="n">
         <v>0</v>
       </c>
+      <c r="T138" t="inlineStr">
+        <is>
+          <t>Union City, TN</t>
+        </is>
+      </c>
+      <c r="U138" t="n">
+        <v>11048.05194805195</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -9851,6 +10947,14 @@
       <c r="S139" t="n">
         <v>0</v>
       </c>
+      <c r="T139" t="inlineStr">
+        <is>
+          <t>Maynardville, TN</t>
+        </is>
+      </c>
+      <c r="U139" t="n">
+        <v>6104.394679238929</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -9920,6 +11024,14 @@
       <c r="S140" t="n">
         <v>0</v>
       </c>
+      <c r="T140" t="inlineStr">
+        <is>
+          <t>Spencer, TN</t>
+        </is>
+      </c>
+      <c r="U140" t="n">
+        <v>12086.90176322418</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -9989,6 +11101,14 @@
       <c r="S141" t="n">
         <v>0</v>
       </c>
+      <c r="T141" t="inlineStr">
+        <is>
+          <t>McMinnville, TN</t>
+        </is>
+      </c>
+      <c r="U141" t="n">
+        <v>10280.22232515053</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -10056,6 +11176,14 @@
       <c r="S142" t="n">
         <v>0</v>
       </c>
+      <c r="T142" t="inlineStr">
+        <is>
+          <t>Jonesborough, TN</t>
+        </is>
+      </c>
+      <c r="U142" t="n">
+        <v>9638.328704262771</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -10125,6 +11253,14 @@
       <c r="S143" t="n">
         <v>0</v>
       </c>
+      <c r="T143" t="inlineStr">
+        <is>
+          <t>Waynesboro, TN</t>
+        </is>
+      </c>
+      <c r="U143" t="n">
+        <v>10841.8131359852</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -10194,6 +11330,14 @@
       <c r="S144" t="n">
         <v>0</v>
       </c>
+      <c r="T144" t="inlineStr">
+        <is>
+          <t>Dresden, TN</t>
+        </is>
+      </c>
+      <c r="U144" t="n">
+        <v>9714.321545021319</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -10262,6 +11406,14 @@
       </c>
       <c r="S145" t="n">
         <v>0</v>
+      </c>
+      <c r="T145" t="inlineStr">
+        <is>
+          <t>Atwood, TN</t>
+        </is>
+      </c>
+      <c r="U145" t="n">
+        <v>10745.51971326165</v>
       </c>
     </row>
     <row r="146">
@@ -10308,6 +11460,12 @@
       <c r="Q146" t="inlineStr"/>
       <c r="R146" t="inlineStr"/>
       <c r="S146" t="inlineStr"/>
+      <c r="T146" t="inlineStr">
+        <is>
+          <t>Jackson, TN</t>
+        </is>
+      </c>
+      <c r="U146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -10377,6 +11535,14 @@
       <c r="S147" t="n">
         <v>0</v>
       </c>
+      <c r="T147" t="inlineStr">
+        <is>
+          <t>Sparta, TN</t>
+        </is>
+      </c>
+      <c r="U147" t="n">
+        <v>13715.39256198347</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -10446,6 +11612,14 @@
       <c r="S148" t="n">
         <v>0</v>
       </c>
+      <c r="T148" t="inlineStr">
+        <is>
+          <t>Franklin, TN</t>
+        </is>
+      </c>
+      <c r="U148" t="n">
+        <v>11580.25657442318</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -10512,6 +11686,14 @@
       <c r="R149" t="inlineStr"/>
       <c r="S149" t="n">
         <v>0</v>
+      </c>
+      <c r="T149" t="inlineStr">
+        <is>
+          <t>Lebanon, TN</t>
+        </is>
+      </c>
+      <c r="U149" t="n">
+        <v>10071.15422493599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>